<commit_message>
- switched off emulate_prepares, thus had to duplicate a lot of param bindings - fixed an issue with positions and surveys in runs, still not too intuitive..
</commit_message>
<xml_diff>
--- a/documentation/Example files/Tagebuch_upload.xlsx
+++ b/documentation/Example files/Tagebuch_upload.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="25035" windowHeight="14865" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="25040" windowHeight="14860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="204">
   <si>
     <t>optional</t>
   </si>
@@ -319,22 +324,6 @@
   </si>
   <si>
     <t>submit_contacts3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sehr zufrieden
-</t>
-  </si>
-  <si>
-    <t>ziemlich zufrieden</t>
-  </si>
-  <si>
-    <t>weder zufrieden noch unzufrieden</t>
-  </si>
-  <si>
-    <t>ziemlich unzufrieden</t>
-  </si>
-  <si>
-    <t>sehr unzufrieden</t>
   </si>
   <si>
     <t>Weiter geht's!</t>
@@ -644,12 +633,33 @@
     <t>Erst einmal geht es um die Personen, __die in Deutschland leben__! Wie häufig hattest du Kontakt mit dieser Person (oder Personengruppe) in den letzten 3 Tagen?
 Wenn du z.B. an allen 3 Tagen Kontakt mit einem oder mehreren Mitschülern hattest, dann klick bitte unter Mitschüler/innen "alle 3 Tage" an.</t>
   </si>
+  <si>
+    <t>hide_label mc-width80 mc-boxed</t>
+  </si>
+  <si>
+    <t>mc-width80 mc-boxed</t>
+  </si>
+  <si>
+    <t>&lt;small&gt;sehr zufrieden&lt;/small&gt;</t>
+  </si>
+  <si>
+    <t>&lt;small&gt;ziemlich zufrieden&lt;/small&gt;</t>
+  </si>
+  <si>
+    <t>&lt;small&gt;weder zufrieden noch unzufrieden&lt;/small&gt;</t>
+  </si>
+  <si>
+    <t>&lt;small&gt;ziemlich unzufrieden&lt;/small&gt;</t>
+  </si>
+  <si>
+    <t>&lt;small&gt;sehr unzufrieden&lt;/small&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -748,6 +758,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -766,8 +792,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -835,8 +863,10 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1240,28 +1270,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="43.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.25" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="21.25" style="2" customWidth="1"/>
-    <col min="11" max="11" width="17.875" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="10.875" style="2"/>
+    <col min="3" max="3" width="13.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="43.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="18.75">
       <c r="A1" s="22" t="s">
         <v>4</v>
       </c>
@@ -1305,18 +1335,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="21" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="21" customFormat="1" ht="409.5">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="18" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
@@ -1327,18 +1357,18 @@
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
     </row>
-    <row r="3" spans="1:14" s="21" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="21" customFormat="1" ht="141.75">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="18" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
@@ -1349,16 +1379,16 @@
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
     </row>
-    <row r="4" spans="1:14" s="7" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="7" customFormat="1" ht="31.5">
       <c r="A4" s="13"/>
       <c r="B4" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="16" t="s">
@@ -1379,10 +1409,10 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>18</v>
@@ -1392,7 +1422,7 @@
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>24</v>
@@ -1409,10 +1439,10 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A6" s="13"/>
       <c r="B6" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>18</v>
@@ -1422,7 +1452,7 @@
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>24</v>
@@ -1439,10 +1469,10 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>18</v>
@@ -1452,7 +1482,7 @@
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>24</v>
@@ -1469,10 +1499,10 @@
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
     </row>
-    <row r="8" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>18</v>
@@ -1482,7 +1512,7 @@
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>24</v>
@@ -1499,10 +1529,10 @@
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
     </row>
-    <row r="9" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>18</v>
@@ -1512,7 +1542,7 @@
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>24</v>
@@ -1529,10 +1559,10 @@
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
     </row>
-    <row r="10" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A10" s="13"/>
       <c r="B10" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>18</v>
@@ -1542,7 +1572,7 @@
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>24</v>
@@ -1559,10 +1589,10 @@
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
     </row>
-    <row r="11" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A11" s="13"/>
       <c r="B11" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>18</v>
@@ -1572,7 +1602,7 @@
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>24</v>
@@ -1589,10 +1619,10 @@
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
     </row>
-    <row r="12" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>18</v>
@@ -1602,7 +1632,7 @@
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>24</v>
@@ -1619,14 +1649,14 @@
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
     </row>
-    <row r="13" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="29" customFormat="1">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17" t="s">
@@ -1641,7 +1671,7 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
     </row>
-    <row r="14" spans="1:14" s="29" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="29" customFormat="1" ht="141.75">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17" t="s">
@@ -1652,7 +1682,7 @@
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="17" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -1663,16 +1693,16 @@
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
     </row>
-    <row r="15" spans="1:14" s="7" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="7" customFormat="1" ht="31.5">
       <c r="A15" s="13"/>
       <c r="B15" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="16" t="s">
@@ -1693,10 +1723,10 @@
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
     </row>
-    <row r="16" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A16" s="13"/>
       <c r="B16" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>18</v>
@@ -1706,7 +1736,7 @@
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="24" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>24</v>
@@ -1723,10 +1753,10 @@
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
     </row>
-    <row r="17" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A17" s="13"/>
       <c r="B17" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>18</v>
@@ -1736,7 +1766,7 @@
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>24</v>
@@ -1753,10 +1783,10 @@
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
     </row>
-    <row r="18" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A18" s="13"/>
       <c r="B18" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>18</v>
@@ -1766,7 +1796,7 @@
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>24</v>
@@ -1783,10 +1813,10 @@
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
     </row>
-    <row r="19" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A19" s="13"/>
       <c r="B19" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>18</v>
@@ -1796,7 +1826,7 @@
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>24</v>
@@ -1813,10 +1843,10 @@
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
     </row>
-    <row r="20" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A20" s="13"/>
       <c r="B20" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>18</v>
@@ -1826,7 +1856,7 @@
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>24</v>
@@ -1843,10 +1873,10 @@
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
     </row>
-    <row r="21" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A21" s="13"/>
       <c r="B21" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>18</v>
@@ -1856,7 +1886,7 @@
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>24</v>
@@ -1873,10 +1903,10 @@
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
     </row>
-    <row r="22" spans="1:14" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="7" customFormat="1" ht="47.25">
       <c r="A22" s="25"/>
       <c r="B22" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>18</v>
@@ -1886,7 +1916,7 @@
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>24</v>
@@ -1903,10 +1933,10 @@
       <c r="M22" s="13"/>
       <c r="N22" s="13"/>
     </row>
-    <row r="23" spans="1:14" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="7" customFormat="1" ht="27" customHeight="1">
       <c r="A23" s="13"/>
       <c r="B23" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>18</v>
@@ -1916,7 +1946,7 @@
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>24</v>
@@ -1933,14 +1963,14 @@
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
     </row>
-    <row r="24" spans="1:14" s="29" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="29" customFormat="1" ht="27" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17" t="s">
@@ -1955,7 +1985,7 @@
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
     </row>
-    <row r="25" spans="1:14" s="17" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="17" customFormat="1" ht="16" customHeight="1">
       <c r="C25" s="17" t="s">
         <v>30</v>
       </c>
@@ -1966,7 +1996,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="21" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="21" customFormat="1" ht="110.25">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17" t="s">
@@ -1975,7 +2005,7 @@
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="18" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
@@ -1986,10 +2016,10 @@
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
     </row>
-    <row r="27" spans="1:14" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="8" customFormat="1" ht="45">
       <c r="A27" s="26"/>
       <c r="B27" s="13" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>17</v>
@@ -2011,7 +2041,7 @@
         <v>33</v>
       </c>
       <c r="J27" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K27" s="26" t="s">
         <v>34</v>
@@ -2026,10 +2056,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>18</v>
@@ -2039,7 +2069,7 @@
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>32</v>
@@ -2051,7 +2081,7 @@
         <v>33</v>
       </c>
       <c r="J28" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K28" s="26" t="s">
         <v>34</v>
@@ -2066,10 +2096,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:14" s="6" customFormat="1" ht="51">
       <c r="A29" s="27"/>
       <c r="B29" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>18</v>
@@ -2079,7 +2109,7 @@
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>32</v>
@@ -2091,7 +2121,7 @@
         <v>33</v>
       </c>
       <c r="J29" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K29" s="26" t="s">
         <v>34</v>
@@ -2106,10 +2136,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>18</v>
@@ -2119,7 +2149,7 @@
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>32</v>
@@ -2131,7 +2161,7 @@
         <v>33</v>
       </c>
       <c r="J30" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K30" s="26" t="s">
         <v>34</v>
@@ -2146,10 +2176,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>18</v>
@@ -2159,7 +2189,7 @@
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>32</v>
@@ -2171,7 +2201,7 @@
         <v>33</v>
       </c>
       <c r="J31" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K31" s="26" t="s">
         <v>34</v>
@@ -2186,10 +2216,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>18</v>
@@ -2199,7 +2229,7 @@
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>32</v>
@@ -2211,7 +2241,7 @@
         <v>33</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K32" s="26" t="s">
         <v>34</v>
@@ -2226,10 +2256,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>18</v>
@@ -2239,7 +2269,7 @@
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>32</v>
@@ -2251,7 +2281,7 @@
         <v>33</v>
       </c>
       <c r="J33" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K33" s="26" t="s">
         <v>34</v>
@@ -2266,10 +2296,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>18</v>
@@ -2279,7 +2309,7 @@
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>32</v>
@@ -2291,7 +2321,7 @@
         <v>33</v>
       </c>
       <c r="J34" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K34" s="26" t="s">
         <v>34</v>
@@ -2306,10 +2336,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>18</v>
@@ -2319,7 +2349,7 @@
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>32</v>
@@ -2331,7 +2361,7 @@
         <v>33</v>
       </c>
       <c r="J35" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K35" s="26" t="s">
         <v>34</v>
@@ -2346,10 +2376,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="6" customFormat="1" ht="30">
       <c r="A36" s="13"/>
       <c r="B36" s="13" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>28</v>
@@ -2367,7 +2397,7 @@
       </c>
       <c r="I36" s="26"/>
       <c r="J36" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
@@ -2378,10 +2408,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>17</v>
@@ -2403,7 +2433,7 @@
         <v>33</v>
       </c>
       <c r="J37" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K37" s="26" t="s">
         <v>34</v>
@@ -2418,10 +2448,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>18</v>
@@ -2431,7 +2461,7 @@
       </c>
       <c r="E38" s="13"/>
       <c r="F38" s="24" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>32</v>
@@ -2443,7 +2473,7 @@
         <v>33</v>
       </c>
       <c r="J38" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K38" s="26" t="s">
         <v>34</v>
@@ -2458,10 +2488,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>18</v>
@@ -2471,7 +2501,7 @@
       </c>
       <c r="E39" s="13"/>
       <c r="F39" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>32</v>
@@ -2483,7 +2513,7 @@
         <v>33</v>
       </c>
       <c r="J39" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K39" s="26" t="s">
         <v>34</v>
@@ -2498,10 +2528,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>18</v>
@@ -2511,7 +2541,7 @@
       </c>
       <c r="E40" s="13"/>
       <c r="F40" s="13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>32</v>
@@ -2523,7 +2553,7 @@
         <v>33</v>
       </c>
       <c r="J40" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K40" s="26" t="s">
         <v>34</v>
@@ -2538,10 +2568,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>18</v>
@@ -2551,7 +2581,7 @@
       </c>
       <c r="E41" s="13"/>
       <c r="F41" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>32</v>
@@ -2563,7 +2593,7 @@
         <v>33</v>
       </c>
       <c r="J41" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K41" s="26" t="s">
         <v>34</v>
@@ -2578,10 +2608,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>18</v>
@@ -2591,7 +2621,7 @@
       </c>
       <c r="E42" s="13"/>
       <c r="F42" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>32</v>
@@ -2603,7 +2633,7 @@
         <v>33</v>
       </c>
       <c r="J42" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K42" s="26" t="s">
         <v>34</v>
@@ -2618,10 +2648,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>18</v>
@@ -2631,7 +2661,7 @@
       </c>
       <c r="E43" s="13"/>
       <c r="F43" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>32</v>
@@ -2643,7 +2673,7 @@
         <v>33</v>
       </c>
       <c r="J43" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K43" s="26" t="s">
         <v>34</v>
@@ -2658,10 +2688,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="6" customFormat="1" ht="47.25">
       <c r="A44" s="25"/>
       <c r="B44" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>18</v>
@@ -2671,7 +2701,7 @@
       </c>
       <c r="E44" s="13"/>
       <c r="F44" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G44" s="13" t="s">
         <v>32</v>
@@ -2683,7 +2713,7 @@
         <v>33</v>
       </c>
       <c r="J44" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K44" s="26" t="s">
         <v>34</v>
@@ -2698,10 +2728,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="6" customFormat="1" ht="27" customHeight="1">
       <c r="A45" s="13"/>
       <c r="B45" s="13" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>18</v>
@@ -2711,7 +2741,7 @@
       </c>
       <c r="E45" s="13"/>
       <c r="F45" s="13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G45" s="13" t="s">
         <v>32</v>
@@ -2723,7 +2753,7 @@
         <v>33</v>
       </c>
       <c r="J45" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K45" s="26" t="s">
         <v>34</v>
@@ -2738,7 +2768,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="17" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" s="17" customFormat="1" ht="16" customHeight="1">
       <c r="C46" s="17" t="s">
         <v>30</v>
       </c>
@@ -2756,7 +2786,7 @@
       <c r="M46" s="20"/>
       <c r="N46" s="20"/>
     </row>
-    <row r="47" spans="1:14" s="21" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" s="21" customFormat="1" ht="141.75">
       <c r="A47" s="17"/>
       <c r="B47" s="17"/>
       <c r="C47" s="17" t="s">
@@ -2765,7 +2795,7 @@
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
       <c r="F47" s="18" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
@@ -2776,10 +2806,10 @@
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
     </row>
-    <row r="48" spans="1:14" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" s="10" customFormat="1" ht="30">
       <c r="A48" s="26"/>
       <c r="B48" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C48" s="26" t="s">
         <v>17</v>
@@ -2791,29 +2821,29 @@
       <c r="F48" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G48" s="26" t="s">
-        <v>101</v>
+      <c r="G48" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="H48" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I48" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J48" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K48" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L48" s="26"/>
       <c r="M48" s="26"/>
       <c r="N48" s="26"/>
     </row>
-    <row r="49" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A49" s="13"/>
       <c r="B49" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>18</v>
@@ -2823,31 +2853,31 @@
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="G49" s="26" t="s">
-        <v>101</v>
+        <v>145</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="H49" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I49" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J49" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K49" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L49" s="13"/>
       <c r="M49" s="13"/>
       <c r="N49" s="13"/>
     </row>
-    <row r="50" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A50" s="13"/>
       <c r="B50" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>18</v>
@@ -2857,31 +2887,31 @@
       </c>
       <c r="E50" s="13"/>
       <c r="F50" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="G50" s="26" t="s">
-        <v>101</v>
+        <v>146</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I50" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J50" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K50" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L50" s="13"/>
       <c r="M50" s="13"/>
       <c r="N50" s="13"/>
     </row>
-    <row r="51" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A51" s="13"/>
       <c r="B51" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>18</v>
@@ -2891,31 +2921,31 @@
       </c>
       <c r="E51" s="13"/>
       <c r="F51" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="G51" s="26" t="s">
-        <v>101</v>
+        <v>147</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="H51" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I51" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J51" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K51" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L51" s="13"/>
       <c r="M51" s="13"/>
       <c r="N51" s="13"/>
     </row>
-    <row r="52" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A52" s="13"/>
       <c r="B52" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>18</v>
@@ -2925,31 +2955,31 @@
       </c>
       <c r="E52" s="13"/>
       <c r="F52" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="G52" s="26" t="s">
-        <v>101</v>
+        <v>148</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="H52" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I52" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J52" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K52" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L52" s="13"/>
       <c r="M52" s="13"/>
       <c r="N52" s="13"/>
     </row>
-    <row r="53" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A53" s="13"/>
       <c r="B53" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>18</v>
@@ -2959,31 +2989,31 @@
       </c>
       <c r="E53" s="13"/>
       <c r="F53" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="G53" s="26" t="s">
-        <v>101</v>
+        <v>149</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I53" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J53" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K53" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L53" s="13"/>
       <c r="M53" s="13"/>
       <c r="N53" s="13"/>
     </row>
-    <row r="54" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A54" s="13"/>
       <c r="B54" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>18</v>
@@ -2993,31 +3023,31 @@
       </c>
       <c r="E54" s="13"/>
       <c r="F54" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="G54" s="26" t="s">
-        <v>101</v>
+        <v>150</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I54" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J54" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K54" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L54" s="13"/>
       <c r="M54" s="13"/>
       <c r="N54" s="13"/>
     </row>
-    <row r="55" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A55" s="13"/>
       <c r="B55" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>18</v>
@@ -3027,31 +3057,31 @@
       </c>
       <c r="E55" s="13"/>
       <c r="F55" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="G55" s="26" t="s">
-        <v>101</v>
+        <v>151</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I55" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J55" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K55" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L55" s="13"/>
       <c r="M55" s="13"/>
       <c r="N55" s="13"/>
     </row>
-    <row r="56" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A56" s="13"/>
       <c r="B56" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>18</v>
@@ -3061,31 +3091,31 @@
       </c>
       <c r="E56" s="13"/>
       <c r="F56" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="G56" s="26" t="s">
-        <v>101</v>
+        <v>152</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I56" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J56" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K56" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L56" s="13"/>
       <c r="M56" s="13"/>
       <c r="N56" s="13"/>
     </row>
-    <row r="57" spans="1:14" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" s="9" customFormat="1" ht="31.5">
       <c r="A57" s="13"/>
       <c r="B57" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>28</v>
@@ -3106,10 +3136,10 @@
       <c r="M57" s="13"/>
       <c r="N57" s="13"/>
     </row>
-    <row r="58" spans="1:14" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" s="9" customFormat="1" ht="30">
       <c r="A58" s="13"/>
       <c r="B58" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>17</v>
@@ -3122,28 +3152,28 @@
         <v>27</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I58" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J58" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K58" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L58" s="13"/>
       <c r="M58" s="13"/>
       <c r="N58" s="13"/>
     </row>
-    <row r="59" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" s="9" customFormat="1" ht="47.25">
       <c r="A59" s="13"/>
       <c r="B59" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>18</v>
@@ -3153,31 +3183,31 @@
       </c>
       <c r="E59" s="13"/>
       <c r="F59" s="24" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I59" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J59" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K59" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L59" s="13"/>
       <c r="M59" s="13"/>
       <c r="N59" s="13"/>
     </row>
-    <row r="60" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" s="9" customFormat="1" ht="47.25">
       <c r="A60" s="13"/>
       <c r="B60" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>18</v>
@@ -3187,31 +3217,31 @@
       </c>
       <c r="E60" s="13"/>
       <c r="F60" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G60" s="26" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I60" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J60" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K60" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L60" s="13"/>
       <c r="M60" s="13"/>
       <c r="N60" s="13"/>
     </row>
-    <row r="61" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" s="9" customFormat="1" ht="47.25">
       <c r="A61" s="13"/>
       <c r="B61" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>18</v>
@@ -3221,31 +3251,31 @@
       </c>
       <c r="E61" s="13"/>
       <c r="F61" s="13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G61" s="26" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="H61" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I61" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J61" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K61" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L61" s="13"/>
       <c r="M61" s="13"/>
       <c r="N61" s="13"/>
     </row>
-    <row r="62" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" s="9" customFormat="1" ht="47.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>18</v>
@@ -3255,31 +3285,31 @@
       </c>
       <c r="E62" s="13"/>
       <c r="F62" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G62" s="26" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="H62" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I62" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J62" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K62" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L62" s="13"/>
       <c r="M62" s="13"/>
       <c r="N62" s="13"/>
     </row>
-    <row r="63" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" s="9" customFormat="1" ht="47.25">
       <c r="A63" s="13"/>
       <c r="B63" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>18</v>
@@ -3289,31 +3319,31 @@
       </c>
       <c r="E63" s="13"/>
       <c r="F63" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G63" s="26" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="H63" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I63" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J63" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K63" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L63" s="13"/>
       <c r="M63" s="13"/>
       <c r="N63" s="13"/>
     </row>
-    <row r="64" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" s="9" customFormat="1" ht="47.25">
       <c r="A64" s="13"/>
       <c r="B64" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>18</v>
@@ -3323,31 +3353,31 @@
       </c>
       <c r="E64" s="13"/>
       <c r="F64" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G64" s="26" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="H64" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I64" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J64" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K64" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L64" s="13"/>
       <c r="M64" s="13"/>
       <c r="N64" s="13"/>
     </row>
-    <row r="65" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" s="9" customFormat="1" ht="47.25">
       <c r="A65" s="25"/>
       <c r="B65" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>18</v>
@@ -3357,31 +3387,31 @@
       </c>
       <c r="E65" s="13"/>
       <c r="F65" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G65" s="26" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="H65" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I65" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J65" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K65" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L65" s="13"/>
       <c r="M65" s="13"/>
       <c r="N65" s="13"/>
     </row>
-    <row r="66" spans="1:14" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" s="9" customFormat="1" ht="27" customHeight="1">
       <c r="A66" s="13"/>
       <c r="B66" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>18</v>
@@ -3391,28 +3421,28 @@
       </c>
       <c r="E66" s="13"/>
       <c r="F66" s="13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G66" s="26" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="H66" s="26" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="I66" s="26" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="J66" s="26" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K66" s="26" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L66" s="13"/>
       <c r="M66" s="13"/>
       <c r="N66" s="13"/>
     </row>
-    <row r="67" spans="1:14" s="17" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" s="17" customFormat="1" ht="16" customHeight="1">
       <c r="C67" s="17" t="s">
         <v>30</v>
       </c>
@@ -3420,10 +3450,10 @@
         <v>100</v>
       </c>
       <c r="F67" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" s="21" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" s="21" customFormat="1" ht="157.5">
       <c r="A68" s="17"/>
       <c r="B68" s="17"/>
       <c r="C68" s="17" t="s">
@@ -3432,7 +3462,7 @@
       <c r="D68" s="17"/>
       <c r="E68" s="17"/>
       <c r="F68" s="18" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G68" s="17"/>
       <c r="H68" s="17"/>
@@ -3443,322 +3473,322 @@
       <c r="M68" s="17"/>
       <c r="N68" s="17"/>
     </row>
-    <row r="69" spans="1:14" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" s="11" customFormat="1" ht="30">
       <c r="A69" s="26"/>
       <c r="B69" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C69" s="26" t="s">
         <v>17</v>
       </c>
       <c r="D69" s="26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E69" s="26"/>
       <c r="F69" s="16" t="s">
         <v>27</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I69" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J69" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K69" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L69" s="26"/>
       <c r="M69" s="26"/>
       <c r="N69" s="26"/>
     </row>
-    <row r="70" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A70" s="13"/>
       <c r="B70" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C70" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E70" s="13"/>
       <c r="F70" s="24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I70" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J70" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K70" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L70" s="13"/>
       <c r="M70" s="13"/>
       <c r="N70" s="13"/>
     </row>
-    <row r="71" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A71" s="13"/>
       <c r="B71" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C71" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E71" s="13"/>
       <c r="F71" s="13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I71" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J71" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K71" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L71" s="13"/>
       <c r="M71" s="13"/>
       <c r="N71" s="13"/>
     </row>
-    <row r="72" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A72" s="13"/>
       <c r="B72" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C72" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E72" s="13"/>
       <c r="F72" s="13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I72" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J72" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K72" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L72" s="13"/>
       <c r="M72" s="13"/>
       <c r="N72" s="13"/>
     </row>
-    <row r="73" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A73" s="13"/>
       <c r="B73" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C73" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E73" s="13"/>
       <c r="F73" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I73" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J73" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K73" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L73" s="13"/>
       <c r="M73" s="13"/>
       <c r="N73" s="13"/>
     </row>
-    <row r="74" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A74" s="13"/>
       <c r="B74" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E74" s="13"/>
       <c r="F74" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I74" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J74" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K74" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L74" s="13"/>
       <c r="M74" s="13"/>
       <c r="N74" s="13"/>
     </row>
-    <row r="75" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A75" s="13"/>
       <c r="B75" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E75" s="13"/>
       <c r="F75" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I75" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J75" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K75" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L75" s="13"/>
       <c r="M75" s="13"/>
       <c r="N75" s="13"/>
     </row>
-    <row r="76" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A76" s="13"/>
       <c r="B76" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E76" s="13"/>
       <c r="F76" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I76" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J76" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K76" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L76" s="13"/>
       <c r="M76" s="13"/>
       <c r="N76" s="13"/>
     </row>
-    <row r="77" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A77" s="13"/>
       <c r="B77" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E77" s="13"/>
       <c r="F77" s="13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I77" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J77" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K77" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L77" s="13"/>
       <c r="M77" s="13"/>
       <c r="N77" s="13"/>
     </row>
-    <row r="78" spans="1:14" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" s="12" customFormat="1" ht="31.5">
       <c r="A78" s="13"/>
       <c r="B78" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E78" s="13"/>
       <c r="F78" s="13" t="s">
@@ -3773,324 +3803,324 @@
       <c r="M78" s="13"/>
       <c r="N78" s="13"/>
     </row>
-    <row r="79" spans="1:14" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" s="12" customFormat="1" ht="31.5">
       <c r="A79" s="13"/>
       <c r="B79" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C79" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E79" s="13"/>
       <c r="F79" s="16" t="s">
         <v>27</v>
       </c>
       <c r="G79" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I79" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J79" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K79" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L79" s="13"/>
       <c r="M79" s="13"/>
       <c r="N79" s="13"/>
     </row>
-    <row r="80" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A80" s="13"/>
       <c r="B80" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E80" s="13"/>
       <c r="F80" s="24" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G80" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I80" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J80" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K80" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L80" s="13"/>
       <c r="M80" s="13"/>
       <c r="N80" s="13"/>
     </row>
-    <row r="81" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A81" s="13"/>
       <c r="B81" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E81" s="13"/>
       <c r="F81" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G81" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I81" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J81" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K81" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L81" s="13"/>
       <c r="M81" s="13"/>
       <c r="N81" s="13"/>
     </row>
-    <row r="82" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A82" s="13"/>
       <c r="B82" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E82" s="13"/>
       <c r="F82" s="13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G82" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I82" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J82" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K82" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L82" s="13"/>
       <c r="M82" s="13"/>
       <c r="N82" s="13"/>
     </row>
-    <row r="83" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A83" s="13"/>
       <c r="B83" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E83" s="13"/>
       <c r="F83" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G83" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I83" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J83" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K83" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L83" s="13"/>
       <c r="M83" s="13"/>
       <c r="N83" s="13"/>
     </row>
-    <row r="84" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A84" s="13"/>
       <c r="B84" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C84" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E84" s="13"/>
       <c r="F84" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G84" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J84" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K84" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L84" s="13"/>
       <c r="M84" s="13"/>
       <c r="N84" s="13"/>
     </row>
-    <row r="85" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A85" s="13"/>
       <c r="B85" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E85" s="13"/>
       <c r="F85" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I85" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J85" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K85" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L85" s="13"/>
       <c r="M85" s="13"/>
       <c r="N85" s="13"/>
     </row>
-    <row r="86" spans="1:14" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" s="12" customFormat="1" ht="47.25">
       <c r="A86" s="25"/>
       <c r="B86" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C86" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E86" s="13"/>
       <c r="F86" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G86" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I86" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J86" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K86" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L86" s="13"/>
       <c r="M86" s="13"/>
       <c r="N86" s="13"/>
     </row>
-    <row r="87" spans="1:14" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" s="12" customFormat="1" ht="27" customHeight="1">
       <c r="A87" s="13"/>
       <c r="B87" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C87" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E87" s="13"/>
       <c r="F87" s="13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G87" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I87" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J87" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K87" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L87" s="13"/>
       <c r="M87" s="13"/>
       <c r="N87" s="13"/>
     </row>
-    <row r="88" spans="1:14" s="17" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" s="17" customFormat="1" ht="16" customHeight="1">
       <c r="C88" s="17" t="s">
         <v>30</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F88" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" s="21" customFormat="1">
       <c r="A89" s="17"/>
       <c r="B89" s="17"/>
       <c r="C89" s="17" t="s">
@@ -4108,109 +4138,109 @@
       <c r="M89" s="17"/>
       <c r="N89" s="17"/>
     </row>
-    <row r="90" spans="1:14" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" s="14" customFormat="1" ht="31.5">
       <c r="A90" s="26"/>
       <c r="B90" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C90" s="26" t="s">
         <v>17</v>
       </c>
       <c r="D90" s="26" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E90" s="26"/>
       <c r="F90" s="26" t="s">
         <v>29</v>
       </c>
       <c r="G90" s="13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H90" s="28" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I90" s="26" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J90" s="26" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K90" s="26" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="L90" s="26"/>
       <c r="M90" s="26"/>
       <c r="N90" s="26"/>
     </row>
-    <row r="91" spans="1:14" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" s="15" customFormat="1" ht="47.25">
       <c r="A91" s="13"/>
       <c r="B91" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C91" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E91" s="13"/>
       <c r="F91" s="24" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G91" s="13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H91" s="28" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I91" s="26" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J91" s="26" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K91" s="26" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="L91" s="13"/>
       <c r="M91" s="13"/>
       <c r="N91" s="13"/>
     </row>
-    <row r="92" spans="1:14" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" s="15" customFormat="1" ht="47.25">
       <c r="A92" s="13"/>
       <c r="B92" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C92" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E92" s="13"/>
       <c r="F92" s="13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G92" s="13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H92" s="28" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I92" s="26" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J92" s="26" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K92" s="26" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="L92" s="13"/>
       <c r="M92" s="13"/>
       <c r="N92" s="13"/>
     </row>
-    <row r="93" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" s="17" customFormat="1">
       <c r="C93" s="17" t="s">
         <v>28</v>
       </c>
@@ -4219,319 +4249,319 @@
       <c r="J93" s="20"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:14" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" s="13" customFormat="1" ht="31.5">
       <c r="B94" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C94" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F94" s="16" t="s">
         <v>29</v>
       </c>
       <c r="G94" s="13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H94" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I94" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J94" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="K94" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" s="13" customFormat="1" ht="47.25">
+      <c r="B95" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D95" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I94" s="13" t="s">
+      <c r="F95" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G95" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="H95" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I95" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J95" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="K95" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" s="13" customFormat="1" ht="47.25">
+      <c r="B96" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D96" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="J94" s="13" t="s">
+      <c r="F96" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="G96" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="H96" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I96" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J96" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="K96" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" s="13" customFormat="1" ht="47.25">
+      <c r="B97" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D97" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="K94" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B95" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C95" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D95" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="F95" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="G95" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H95" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="I95" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="J95" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="K95" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B96" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C96" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D96" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="F96" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="G96" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="I96" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="J96" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="K96" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B97" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C97" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D97" s="13" t="s">
-        <v>149</v>
-      </c>
       <c r="F97" s="16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G97" s="13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I97" s="13" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="J97" s="13" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" s="17" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" s="17" customFormat="1" ht="63">
       <c r="C98" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D98" s="17" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F98" s="18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" ht="31.5">
       <c r="A99" s="13"/>
       <c r="B99" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C99" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E99" s="13"/>
       <c r="F99" s="16" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G99" s="13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I99" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J99" s="13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L99" s="13"/>
       <c r="M99" s="13"/>
       <c r="N99" s="13"/>
     </row>
-    <row r="100" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="47.25">
       <c r="A100" s="13"/>
       <c r="B100" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C100" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E100" s="13"/>
       <c r="F100" s="16" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G100" s="13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H100" s="13" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I100" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J100" s="13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L100" s="13"/>
       <c r="M100" s="13"/>
       <c r="N100" s="13"/>
     </row>
-    <row r="101" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="47.25">
       <c r="A101" s="13"/>
       <c r="B101" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E101" s="13"/>
       <c r="F101" s="16" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G101" s="13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H101" s="13" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I101" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J101" s="13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K101" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L101" s="13"/>
       <c r="M101" s="13"/>
       <c r="N101" s="13"/>
     </row>
-    <row r="102" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="47.25">
       <c r="A102" s="13"/>
       <c r="B102" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C102" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D102" s="13" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E102" s="13"/>
       <c r="F102" s="16" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G102" s="13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H102" s="13" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I102" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J102" s="13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K102" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L102" s="13"/>
       <c r="M102" s="13"/>
       <c r="N102" s="13"/>
     </row>
-    <row r="103" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="47.25">
       <c r="A103" s="13"/>
       <c r="B103" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C103" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D103" s="13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E103" s="13"/>
       <c r="F103" s="16" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G103" s="13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H103" s="13" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I103" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J103" s="13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K103" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L103" s="13"/>
       <c r="M103" s="13"/>
       <c r="N103" s="13"/>
     </row>
-    <row r="104" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" s="17" customFormat="1">
       <c r="C104" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F104" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" s="21" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" s="21" customFormat="1" ht="141.75">
       <c r="A105" s="17"/>
       <c r="B105" s="17"/>
       <c r="C105" s="17"/>
       <c r="D105" s="17"/>
       <c r="E105" s="17"/>
       <c r="F105" s="18" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G105" s="17"/>
       <c r="H105" s="17"/>
@@ -4542,21 +4572,26 @@
       <c r="M105" s="17"/>
       <c r="N105" s="17"/>
     </row>
-    <row r="106" spans="1:14" s="17" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" s="17" customFormat="1" ht="31.5">
       <c r="C106" s="17" t="s">
         <v>30</v>
       </c>
       <c r="D106" s="17" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F106" s="18" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4569,12 +4604,12 @@
       <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -4586,7 +4621,7 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -4598,7 +4633,7 @@
       </c>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="B3">
         <v>3</v>
       </c>
@@ -4606,7 +4641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="B4">
         <v>4</v>
       </c>
@@ -4614,7 +4649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="B5">
         <v>5</v>
       </c>
@@ -4622,7 +4657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="B6">
         <v>6</v>
       </c>
@@ -4630,7 +4665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="B7">
         <v>7</v>
       </c>
@@ -4638,7 +4673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="B8">
         <v>1</v>
       </c>
@@ -4646,15 +4681,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="C10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>